<commit_message>
wip: work on wound and pressureUlcer zibs
</commit_message>
<xml_diff>
--- a/Mappings/PressureUlcer - STU3.xlsx
+++ b/Mappings/PressureUlcer - STU3.xlsx
@@ -668,16 +668,19 @@
     <t>Condition.code</t>
   </si>
   <si>
-    <t>Observation(pressureUlcurObservable).component.woundLength (valueQuantity, ucum)</t>
-  </si>
-  <si>
-    <t>Observation(pressureUlcurObservable).component.woundWidth (valueQuantity, ucum)</t>
-  </si>
-  <si>
-    <t>Observation(pressureUlcurObservable).component.woundDepth (valueQuantity, ucum)</t>
-  </si>
-  <si>
     <t>Media (resource)</t>
+  </si>
+  <si>
+    <t>Observation(pressureUlcurObservable).component.woundLength (valueQuantity, ucum)
+Referred to the Condition @ .reasonReference (extension)</t>
+  </si>
+  <si>
+    <t>Observation(woundUlcurObservable).component.woundWidth (valueQuantity, ucum)
+Referred to the Condition @ .reasonReference (extension)</t>
+  </si>
+  <si>
+    <t>Observation(woundObservable).component.woundDepth (valueQuantity, ucum)
+Referred to the Condition @ .reasonReference (extension)</t>
   </si>
 </sst>
 </file>
@@ -1058,7 +1061,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1099,7 +1102,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1140,7 +1143,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2941,7 +2944,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4209,8 +4212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4446,7 +4449,7 @@
       <c r="S6" s="3"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="2:20" ht="38.25">
+    <row r="7" spans="2:20" ht="25.5">
       <c r="B7" s="11"/>
       <c r="C7" s="12" t="s">
         <v>100</v>
@@ -4530,7 +4533,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="2:20" ht="25.5">
+    <row r="9" spans="2:20" ht="51">
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
         <v>110</v>
@@ -4562,7 +4565,7 @@
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="15" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="Q9" s="15" t="s">
         <v>183</v>
@@ -4571,7 +4574,7 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="2:20" ht="25.5">
+    <row r="10" spans="2:20" ht="51">
       <c r="B10" s="11"/>
       <c r="C10" s="12" t="s">
         <v>116</v>
@@ -4603,7 +4606,7 @@
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="15" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="Q10" s="15" t="s">
         <v>183</v>
@@ -4612,7 +4615,7 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="2:20" ht="25.5">
+    <row r="11" spans="2:20" ht="51">
       <c r="B11" s="11"/>
       <c r="C11" s="12" t="s">
         <v>121</v>
@@ -4644,7 +4647,7 @@
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="15" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q11" s="15" t="s">
         <v>183</v>
@@ -4685,7 +4688,7 @@
       </c>
       <c r="O12" s="2"/>
       <c r="P12" s="15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="Q12" s="15" t="s">
         <v>183</v>
@@ -5105,6 +5108,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -5295,12 +5304,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43D78D48-D94B-4B76-BF66-2E1C35A17643}">
   <ds:schemaRefs>
@@ -5310,6 +5313,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1334EEF1-4DFB-47DA-9620-E323C8D5F690}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{883326BD-BF9E-494C-975F-7B35DECF4D17}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5326,13 +5338,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1334EEF1-4DFB-47DA-9620-E323C8D5F690}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
wip: Also added profile and valueset for zib-Wound
</commit_message>
<xml_diff>
--- a/Mappings/PressureUlcer - STU3.xlsx
+++ b/Mappings/PressureUlcer - STU3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="615" windowWidth="27495" windowHeight="11955" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="630" yWindow="615" windowWidth="27495" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1061,7 +1061,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1102,7 +1102,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1143,7 +1143,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2944,7 +2944,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2954,7 +2954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -4212,7 +4212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
@@ -5108,12 +5108,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -5304,6 +5298,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43D78D48-D94B-4B76-BF66-2E1C35A17643}">
   <ds:schemaRefs>
@@ -5313,15 +5313,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1334EEF1-4DFB-47DA-9620-E323C8D5F690}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{883326BD-BF9E-494C-975F-7B35DECF4D17}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5338,4 +5329,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1334EEF1-4DFB-47DA-9620-E323C8D5F690}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>